<commit_message>
updated the product template for uploading products
</commit_message>
<xml_diff>
--- a/public/products_template.xlsx
+++ b/public/products_template.xlsx
@@ -19,29 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Pacific</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>1Lorem, ipsum dolor sit amet consectetur adipisicing elit. Deleniti optio nihil sint minima rerum! Minima quod suscipit voluptates quasi sapiente?</t>
   </si>
   <si>
-    <t>3Lorem, ipsum dolor sit amet consectetur adipisicing elit. Deleniti optio nihil sint minima rerum! Minima quod suscipit voluptates quasi sapiente?</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/ALLEGRA_COLLECTION_1.jpg</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/ARAVALLI_COLLECTION_1.jpg</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/category/linnae.jpg</t>
-  </si>
-  <si>
     <t>available</t>
   </si>
   <si>
@@ -54,45 +36,12 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>42348fec-0777-4555-a935-638a57eb33f0</t>
-  </si>
-  <si>
-    <t>cd312b6e-ff18-4f19-b0d5-993d7b091a84</t>
-  </si>
-  <si>
-    <t>7346acda-0f39-4d74-bba5-c92fea872cda</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/SAVONA_COLLECTION_1.jpg</t>
-  </si>
-  <si>
-    <t>e68470cf-fad6-4914-9265-b750d9472f55</t>
-  </si>
-  <si>
-    <t>920afaaa-ec63-46c3-86d5-98383683d62b</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/SAVANNAH_COLLECTION_1.jpg</t>
-  </si>
-  <si>
-    <t>8c947531-325e-46e9-a2a1-4f9c19caf8b3</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/MUSTIQUE_COLLECTION_1.jpg</t>
-  </si>
-  <si>
-    <t>https://ashleywildegroup.com/media/catalog/collection-sm/MIRAGE_COLLECTION_1.jpg</t>
-  </si>
-  <si>
     <t>product_name</t>
   </si>
   <si>
     <t>product_description</t>
   </si>
   <si>
-    <t>category_id</t>
-  </si>
-  <si>
     <t>best_seller</t>
   </si>
   <si>
@@ -114,20 +63,62 @@
     <t>product_image5</t>
   </si>
   <si>
-    <t>size_id</t>
-  </si>
-  <si>
-    <t>color_id</t>
-  </si>
-  <si>
     <t>variation_image</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>category one</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>xL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>3 Lorem, ipsum dolor sit amet consectetur adipisicing elit. Deleniti optio nihil sint minima rerum! Minima quod suscipit voluptates quasi sapiente?</t>
+  </si>
+  <si>
+    <t>Alaska Collection</t>
+  </si>
+  <si>
+    <t>Atlantic Collection</t>
+  </si>
+  <si>
+    <t>category four</t>
+  </si>
+  <si>
+    <t>https://ashleywildegroup.com//media/catalog/category/Cotswolds_Category_1_1.jpg</t>
+  </si>
+  <si>
+    <t>https://ashleywildegroup.com//media/catalog/category/Sirenete_Category.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,20 +132,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF020817"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -206,23 +183,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -232,9 +202,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -540,96 +509,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>11</v>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O2" s="1">
         <v>150</v>
@@ -637,81 +598,56 @@
       <c r="P2" s="1">
         <v>60</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="4" t="s">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3">
+        <v>150</v>
+      </c>
+      <c r="P3">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="1">
-        <v>250</v>
-      </c>
-      <c r="P3" s="1">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="b">
+      <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="O4" s="1">
         <v>500</v>
@@ -719,13 +655,214 @@
       <c r="P4" s="1">
         <v>100</v>
       </c>
-      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="D50" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change size section style in single product page
</commit_message>
<xml_diff>
--- a/public/products_template.xlsx
+++ b/public/products_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="245">
   <si>
     <t>available</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>xs</t>
-  </si>
-  <si>
-    <t>MODERN CLASSICS GRAPHIC TEE</t>
   </si>
   <si>
     <t>&lt;p&gt;MODERN CLASSICS GRAPHIC TEE&lt;br /&gt;Description&lt;br /&gt;A CLASSIC TEE THAT NODS TO THE BRAND WITH THE 3-STRIPES.&lt;br /&gt;A premium look for easygoing days. This adidas tee is made from soft French terry material that keeps you comfortable whether you're out exploring the city or relaxing at home. Embroidery on the front adds subtle texture and retro style. Pair this top with joggers for a sporty vibe or jeans and sneakers for casual weekend adventures. Wherever the day takes you, this tee has you covered in comfort and style.The cotton in this product has been sourced through Better Cotton. Better Cotton is sourced via a chain of custody model called mass balance. This means that Better Cotton is not physically traceable to end products.&lt;br /&gt;Details&lt;br /&gt;Regular fit&lt;br /&gt;Crewneck&lt;br /&gt;70% cotton, 30% polyester (recycled)&lt;br /&gt;Embroidered details&lt;br /&gt;Sourced through Better Cotton via a system of mass balance and therefore this product may not contain Better Cotton&lt;br /&gt;Colour: Black&lt;br /&gt;Product code: IW2705&lt;br /&gt;Care&lt;br /&gt;WASHING INSTRUCTIONS&lt;br /&gt;Do not bleach&lt;br /&gt;Tumble dry low heat&lt;br /&gt;Do not dry clean&lt;br /&gt;Touch up with cool iron&lt;br /&gt;Machine wash warm&lt;br /&gt;EXTRA CARE INFORMATION&lt;br /&gt;Wash with like colors&lt;br /&gt;Wash and iron inside out&lt;br /&gt;Use mild detergent only&lt;/p&gt;</t>
@@ -866,6 +863,15 @@
   </si>
   <si>
     <t>https://media.zid.store/675070ce-1a39-4ad3-8aa5-85b6c78651b3/f58e1a14-3db1-4c7d-923c-b550819202fc.jpg</t>
+  </si>
+  <si>
+    <t>MODERN GRAPHIC lorem</t>
+  </si>
+  <si>
+    <t>https://media.zid.store/675070ce-1a39-4ad3-8aa5-85b6c78651b3/d67c00a7-ecab-4125-b161-ac9d3c887fa9.jpg</t>
+  </si>
+  <si>
+    <t>https://media.zid.store/675070ce-1a39-4ad3-8aa5-85b6c78651b3/27fc398a-719f-4919-8634-052e26fa0389.jpg</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T80"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,10 +1298,10 @@
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
@@ -1304,7 +1310,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -1351,52 +1357,52 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>25</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>17</v>
@@ -1408,15 +1414,15 @@
         <v>32</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>17</v>
@@ -1427,13 +1433,16 @@
       <c r="S3">
         <v>5</v>
       </c>
+      <c r="T3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>17</v>
@@ -1444,13 +1453,16 @@
       <c r="S4">
         <v>7</v>
       </c>
+      <c r="T4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>17</v>
@@ -1461,14 +1473,17 @@
       <c r="S5">
         <v>9</v>
       </c>
+      <c r="T5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="G6" s="1"/>
       <c r="P6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>17</v>
@@ -1479,11 +1494,13 @@
       <c r="S6">
         <v>10</v>
       </c>
-      <c r="T6" s="1"/>
+      <c r="T6" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="P7" t="s">
         <v>20</v>
@@ -1497,642 +1514,561 @@
       <c r="S7">
         <v>10</v>
       </c>
-      <c r="T7" s="1"/>
+      <c r="T7" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" t="s">
-        <v>43</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="1"/>
       <c r="P8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R8">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S8">
-        <v>47</v>
-      </c>
-      <c r="T8" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>242</v>
       </c>
       <c r="P9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R9">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S9">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P10" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R10">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S10">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P11" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R11">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S11">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>242</v>
       </c>
       <c r="G12" s="1"/>
       <c r="P12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R12">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S12">
         <v>10</v>
       </c>
+      <c r="T12" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P13" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="5" t="s">
-        <v>19</v>
+      <c r="Q13" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R13">
-        <v>209</v>
+        <v>279</v>
       </c>
       <c r="S13">
         <v>10</v>
       </c>
+      <c r="T13" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" t="s">
-        <v>50</v>
-      </c>
-      <c r="M14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O14" t="s">
-        <v>53</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="1"/>
       <c r="P14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="R14">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="S14">
-        <v>59</v>
-      </c>
-      <c r="T14" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P15" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="R15">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="S15">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P16" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="R16">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="S16">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>242</v>
+      </c>
       <c r="P17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="R17">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="S17">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="G18" s="1"/>
       <c r="P18" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="R18">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="S18">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" t="s">
-        <v>67</v>
-      </c>
-      <c r="M19" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" t="s">
-        <v>69</v>
-      </c>
-      <c r="O19" t="s">
-        <v>70</v>
+        <v>242</v>
       </c>
       <c r="P19" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="R19">
-        <v>499</v>
+        <v>279</v>
       </c>
       <c r="S19">
-        <v>54</v>
-      </c>
-      <c r="T19" s="6" t="s">
-        <v>72</v>
+        <v>10</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N20" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" t="s">
+        <v>42</v>
+      </c>
       <c r="P20" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>71</v>
+        <v>24</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R20">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S20">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="T20" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>34</v>
+      </c>
       <c r="P21" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>71</v>
+        <v>25</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R21">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S21">
-        <v>56</v>
-      </c>
-      <c r="T21" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G22" s="1"/>
       <c r="P22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R22">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S22">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G23" s="1"/>
       <c r="P23" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R23">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S23">
-        <v>58</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G24" s="1"/>
       <c r="P24" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R24">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S24">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>79</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N25" t="s">
-        <v>82</v>
-      </c>
-      <c r="O25" t="s">
-        <v>83</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G25" s="1"/>
       <c r="P25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R25">
-        <v>499</v>
+        <v>209</v>
       </c>
       <c r="S25">
-        <v>59</v>
-      </c>
-      <c r="T25" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L26" t="s">
+        <v>49</v>
+      </c>
+      <c r="M26" t="s">
+        <v>50</v>
+      </c>
+      <c r="N26" t="s">
+        <v>51</v>
+      </c>
+      <c r="O26" t="s">
+        <v>52</v>
+      </c>
       <c r="P26" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="R26">
-        <v>499</v>
+        <v>299</v>
       </c>
       <c r="S26">
         <v>59</v>
       </c>
-      <c r="T26" s="6" t="s">
-        <v>85</v>
+      <c r="T26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
       <c r="P27" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>78</v>
+        <v>26</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="R27">
-        <v>499</v>
+        <v>299</v>
       </c>
       <c r="S27">
-        <v>59</v>
-      </c>
-      <c r="T27" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
       <c r="P28" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>78</v>
+        <v>27</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="R28">
-        <v>499</v>
+        <v>299</v>
       </c>
       <c r="S28">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
       <c r="P29" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>78</v>
+        <v>28</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="R29">
-        <v>499</v>
+        <v>299</v>
       </c>
       <c r="S29">
-        <v>59</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
       <c r="P30" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>78</v>
+        <v>53</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="R30">
-        <v>499</v>
+        <v>299</v>
       </c>
       <c r="S30">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G31" s="1" t="b">
         <v>1</v>
@@ -2141,864 +2077,595 @@
         <v>1</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="b">
         <v>1</v>
       </c>
       <c r="K31" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="L31" t="s">
-        <v>192</v>
+        <v>66</v>
       </c>
       <c r="M31" t="s">
-        <v>238</v>
+        <v>67</v>
+      </c>
+      <c r="N31" t="s">
+        <v>68</v>
+      </c>
+      <c r="O31" t="s">
+        <v>69</v>
       </c>
       <c r="P31" t="s">
         <v>25</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R31">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="S31">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E32" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="b">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
-        <v>147</v>
-      </c>
-      <c r="L32" t="s">
-        <v>193</v>
-      </c>
-      <c r="M32" t="s">
-        <v>239</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G32" s="1"/>
       <c r="P32" t="s">
         <v>26</v>
       </c>
-      <c r="Q32" s="5" t="s">
-        <v>71</v>
+      <c r="Q32" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="R32">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="S32">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="T32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D33" t="s">
-        <v>139</v>
-      </c>
-      <c r="E33" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" t="s">
-        <v>148</v>
-      </c>
-      <c r="L33" t="s">
-        <v>194</v>
-      </c>
-      <c r="M33" t="s">
-        <v>240</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="P33" t="s">
         <v>27</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="R33">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="S33">
+        <v>56</v>
+      </c>
+      <c r="T33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" t="b">
-        <v>1</v>
-      </c>
-      <c r="K34" t="s">
-        <v>149</v>
-      </c>
-      <c r="L34" t="s">
-        <v>195</v>
-      </c>
-      <c r="M34" t="s">
-        <v>241</v>
-      </c>
+      <c r="G34" s="1"/>
       <c r="P34" t="s">
         <v>28</v>
       </c>
-      <c r="Q34" s="5" t="s">
-        <v>78</v>
+      <c r="Q34" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="R34">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="S34">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" t="b">
-        <v>1</v>
-      </c>
-      <c r="K35" t="s">
-        <v>150</v>
-      </c>
-      <c r="L35" t="s">
-        <v>196</v>
-      </c>
-      <c r="M35" t="s">
-        <v>242</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G35" s="1"/>
       <c r="P35" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="R35">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="S35">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K36" t="s">
-        <v>151</v>
-      </c>
-      <c r="L36" t="s">
-        <v>197</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G36" s="1"/>
       <c r="P36" t="s">
         <v>20</v>
       </c>
       <c r="Q36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R36">
+        <v>499</v>
+      </c>
+      <c r="S36">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
         <v>78</v>
       </c>
-      <c r="R36">
-        <v>505</v>
-      </c>
-      <c r="S36">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K37" t="s">
-        <v>152</v>
-      </c>
-      <c r="L37" t="s">
-        <v>198</v>
+      <c r="L37" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M37" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" t="s">
+        <v>81</v>
+      </c>
+      <c r="O37" t="s">
+        <v>82</v>
       </c>
       <c r="P37" t="s">
         <v>25</v>
       </c>
-      <c r="Q37" s="5" t="s">
-        <v>71</v>
+      <c r="Q37" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R37">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="S37">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="T37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" t="s">
-        <v>133</v>
-      </c>
-      <c r="D38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="s">
-        <v>153</v>
-      </c>
-      <c r="L38" t="s">
-        <v>199</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
       <c r="P38" t="s">
         <v>26</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R38">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="S38">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" t="s">
-        <v>140</v>
-      </c>
-      <c r="E39" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" t="s">
-        <v>48</v>
-      </c>
-      <c r="G39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" t="b">
-        <v>1</v>
-      </c>
-      <c r="K39" t="s">
-        <v>154</v>
-      </c>
-      <c r="L39" t="s">
-        <v>200</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
       <c r="P39" t="s">
         <v>27</v>
       </c>
-      <c r="Q39" s="5" t="s">
-        <v>78</v>
+      <c r="Q39" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R39">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="S39">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="T39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" t="b">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>155</v>
-      </c>
-      <c r="L40" t="s">
-        <v>201</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
       <c r="P40" t="s">
         <v>28</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="R40">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="S40">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" t="s">
-        <v>140</v>
-      </c>
-      <c r="E41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" t="b">
-        <v>1</v>
-      </c>
-      <c r="K41" t="s">
-        <v>156</v>
-      </c>
-      <c r="L41" t="s">
-        <v>202</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
       <c r="P41" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R41">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="S41">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" t="s">
-        <v>140</v>
-      </c>
-      <c r="E42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" t="b">
-        <v>0</v>
-      </c>
-      <c r="I42" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" t="s">
-        <v>157</v>
-      </c>
-      <c r="L42" t="s">
-        <v>203</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
       <c r="P42" t="s">
         <v>20</v>
       </c>
-      <c r="Q42" s="5" t="s">
-        <v>71</v>
+      <c r="Q42" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R42">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="S42">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="s">
+        <v>145</v>
+      </c>
+      <c r="L43" t="s">
+        <v>191</v>
+      </c>
+      <c r="M43" t="s">
+        <v>237</v>
+      </c>
+      <c r="P43" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R43">
+        <v>500</v>
+      </c>
+      <c r="S43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" t="s">
+        <v>138</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" t="s">
         <v>37</v>
       </c>
-      <c r="F43" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" t="b">
-        <v>1</v>
-      </c>
-      <c r="K43" t="s">
-        <v>158</v>
-      </c>
-      <c r="L43" t="s">
-        <v>204</v>
-      </c>
-      <c r="P43" t="s">
+      <c r="G44" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>146</v>
+      </c>
+      <c r="L44" t="s">
+        <v>192</v>
+      </c>
+      <c r="M44" t="s">
+        <v>238</v>
+      </c>
+      <c r="P44" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="R44">
+        <v>501</v>
+      </c>
+      <c r="S44">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>147</v>
+      </c>
+      <c r="L45" t="s">
+        <v>193</v>
+      </c>
+      <c r="M45" t="s">
+        <v>239</v>
+      </c>
+      <c r="P45" t="s">
         <v>26</v>
       </c>
-      <c r="Q43" s="2" t="s">
+      <c r="Q45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R43">
-        <v>512</v>
-      </c>
-      <c r="S43">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="R45">
+        <v>502</v>
+      </c>
+      <c r="S45">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" t="s">
         <v>23</v>
       </c>
-      <c r="F44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G44" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" t="b">
-        <v>1</v>
-      </c>
-      <c r="J44" t="b">
-        <v>1</v>
-      </c>
-      <c r="K44" t="s">
-        <v>159</v>
-      </c>
-      <c r="L44" t="s">
-        <v>205</v>
-      </c>
-      <c r="P44" t="s">
+      <c r="G46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="s">
+        <v>148</v>
+      </c>
+      <c r="L46" t="s">
+        <v>194</v>
+      </c>
+      <c r="M46" t="s">
+        <v>240</v>
+      </c>
+      <c r="P46" t="s">
         <v>27</v>
       </c>
-      <c r="Q44" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="R44">
-        <v>513</v>
-      </c>
-      <c r="S44">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="s">
-        <v>160</v>
-      </c>
-      <c r="L45" t="s">
-        <v>206</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="Q46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R46">
+        <v>503</v>
+      </c>
+      <c r="S46">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="s">
+        <v>149</v>
+      </c>
+      <c r="L47" t="s">
+        <v>195</v>
+      </c>
+      <c r="M47" t="s">
+        <v>241</v>
+      </c>
+      <c r="P47" t="s">
         <v>28</v>
       </c>
-      <c r="Q45" s="2" t="s">
+      <c r="Q47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R45">
-        <v>514</v>
-      </c>
-      <c r="S45">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" t="s">
-        <v>141</v>
-      </c>
-      <c r="E46" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H46" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" t="b">
-        <v>1</v>
-      </c>
-      <c r="J46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="s">
-        <v>161</v>
-      </c>
-      <c r="L46" t="s">
-        <v>207</v>
-      </c>
-      <c r="P46" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="R46">
-        <v>515</v>
-      </c>
-      <c r="S46">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>103</v>
-      </c>
-      <c r="B47" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" t="s">
-        <v>134</v>
-      </c>
-      <c r="D47" t="s">
-        <v>141</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="R47">
+        <v>504</v>
+      </c>
+      <c r="S47">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" t="s">
         <v>37</v>
       </c>
-      <c r="F47" t="s">
-        <v>48</v>
-      </c>
-      <c r="G47" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J47" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" t="s">
-        <v>162</v>
-      </c>
-      <c r="L47" t="s">
-        <v>208</v>
-      </c>
-      <c r="P47" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="R47">
-        <v>516</v>
-      </c>
-      <c r="S47">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" t="s">
-        <v>38</v>
-      </c>
       <c r="G48" s="1" t="b">
         <v>0</v>
       </c>
@@ -3012,92 +2679,92 @@
         <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="L48" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="P48" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R48">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="S48">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
+        <v>151</v>
+      </c>
+      <c r="L49" t="s">
+        <v>197</v>
+      </c>
+      <c r="P49" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" t="b">
-        <v>1</v>
-      </c>
-      <c r="K49" t="s">
-        <v>164</v>
-      </c>
-      <c r="L49" t="s">
-        <v>210</v>
-      </c>
-      <c r="P49" t="s">
-        <v>27</v>
-      </c>
       <c r="Q49" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R49">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="S49">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E50" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G50" s="1" t="b">
         <v>0</v>
@@ -3112,42 +2779,42 @@
         <v>1</v>
       </c>
       <c r="K50" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="L50" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="P50" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R50">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="S50">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G51" s="1" t="b">
         <v>1</v>
@@ -3162,43 +2829,43 @@
         <v>1</v>
       </c>
       <c r="K51" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="L51" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="P51" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q51" s="2" t="s">
-        <v>78</v>
+        <v>26</v>
+      </c>
+      <c r="Q51" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="R51">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="S51">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" t="s">
         <v>37</v>
       </c>
-      <c r="F52" t="s">
-        <v>38</v>
-      </c>
       <c r="G52" s="1" t="b">
         <v>0</v>
       </c>
@@ -3212,43 +2879,43 @@
         <v>1</v>
       </c>
       <c r="K52" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="L52" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="P52" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q52" s="5" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R52">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="S52">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" t="s">
         <v>23</v>
       </c>
-      <c r="F53" t="s">
-        <v>24</v>
-      </c>
       <c r="G53" s="1" t="b">
         <v>1</v>
       </c>
@@ -3262,43 +2929,43 @@
         <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="L53" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="P53" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R53">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="S53">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E54" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" t="s">
         <v>23</v>
       </c>
-      <c r="F54" t="s">
-        <v>48</v>
-      </c>
       <c r="G54" s="1" t="b">
         <v>0</v>
       </c>
@@ -3312,42 +2979,42 @@
         <v>1</v>
       </c>
       <c r="K54" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="L54" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="P54" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q54" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R54">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="S54">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E55" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F55" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G55" s="1" t="b">
         <v>1</v>
@@ -3362,43 +3029,43 @@
         <v>1</v>
       </c>
       <c r="K55" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="L55" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="P55" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R55">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="S55">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" t="s">
         <v>37</v>
       </c>
-      <c r="F56" t="s">
-        <v>38</v>
-      </c>
       <c r="G56" s="1" t="b">
         <v>0</v>
       </c>
@@ -3412,42 +3079,42 @@
         <v>1</v>
       </c>
       <c r="K56" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="L56" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="P56" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q56" s="2" t="s">
-        <v>78</v>
+        <v>26</v>
+      </c>
+      <c r="Q56" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="R56">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="S56">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E57" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G57" s="1" t="b">
         <v>1</v>
@@ -3462,43 +3129,43 @@
         <v>1</v>
       </c>
       <c r="K57" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="L57" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="P57" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q57" s="5" t="s">
-        <v>71</v>
+        <v>27</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R57">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="S57">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F58" t="s">
         <v>47</v>
       </c>
-      <c r="F58" t="s">
-        <v>24</v>
-      </c>
       <c r="G58" s="1" t="b">
         <v>0</v>
       </c>
@@ -3512,42 +3179,42 @@
         <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="L58" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="P58" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R58">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="S58">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E59" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F59" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G59" s="1" t="b">
         <v>1</v>
@@ -3562,43 +3229,43 @@
         <v>1</v>
       </c>
       <c r="K59" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="L59" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="P59" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="Q59" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R59">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="S59">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>133</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" t="s">
         <v>37</v>
       </c>
-      <c r="F60" t="s">
-        <v>38</v>
-      </c>
       <c r="G60" s="1" t="b">
         <v>0</v>
       </c>
@@ -3612,42 +3279,42 @@
         <v>1</v>
       </c>
       <c r="K60" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="L60" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="P60" t="s">
         <v>25</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R60">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="S60">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E61" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G61" s="1" t="b">
         <v>1</v>
@@ -3662,43 +3329,43 @@
         <v>1</v>
       </c>
       <c r="K61" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="L61" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="P61" t="s">
         <v>26</v>
       </c>
-      <c r="Q61" s="2" t="s">
+      <c r="Q61" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R61">
+        <v>518</v>
+      </c>
+      <c r="S61">
         <v>78</v>
-      </c>
-      <c r="R61">
-        <v>530</v>
-      </c>
-      <c r="S61">
-        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" t="s">
         <v>23</v>
       </c>
-      <c r="F62" t="s">
-        <v>48</v>
-      </c>
       <c r="G62" s="1" t="b">
         <v>0</v>
       </c>
@@ -3712,42 +3379,42 @@
         <v>1</v>
       </c>
       <c r="K62" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="L62" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="P62" t="s">
         <v>27</v>
       </c>
-      <c r="Q62" s="5" t="s">
-        <v>71</v>
+      <c r="Q62" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R62">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="S62">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E63" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F63" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G63" s="1" t="b">
         <v>1</v>
@@ -3762,42 +3429,42 @@
         <v>1</v>
       </c>
       <c r="K63" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="L63" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="P63" t="s">
         <v>28</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R63">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="S63">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E64" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G64" s="1" t="b">
         <v>0</v>
@@ -3812,42 +3479,42 @@
         <v>1</v>
       </c>
       <c r="K64" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="L64" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="P64" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="Q64" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R64">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="S64">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E65" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G65" s="1" t="b">
         <v>1</v>
@@ -3862,43 +3529,43 @@
         <v>1</v>
       </c>
       <c r="K65" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="L65" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="P65" t="s">
         <v>20</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R65">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="S65">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" t="s">
         <v>47</v>
       </c>
-      <c r="F66" t="s">
-        <v>24</v>
-      </c>
       <c r="G66" s="1" t="b">
         <v>0</v>
       </c>
@@ -3912,43 +3579,43 @@
         <v>1</v>
       </c>
       <c r="K66" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="L66" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="P66" t="s">
         <v>25</v>
       </c>
-      <c r="Q66" s="2" t="s">
-        <v>78</v>
+      <c r="Q66" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="R66">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="S66">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" t="s">
         <v>47</v>
       </c>
-      <c r="F67" t="s">
-        <v>38</v>
-      </c>
       <c r="G67" s="1" t="b">
         <v>1</v>
       </c>
@@ -3962,42 +3629,42 @@
         <v>1</v>
       </c>
       <c r="K67" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="L67" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="P67" t="s">
         <v>26</v>
       </c>
-      <c r="Q67" s="5" t="s">
-        <v>71</v>
+      <c r="Q67" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R67">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="S67">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G68" s="1" t="b">
         <v>0</v>
@@ -4012,42 +3679,42 @@
         <v>1</v>
       </c>
       <c r="K68" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="L68" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="P68" t="s">
         <v>27</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R68">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="S68">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D69" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E69" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G69" s="1" t="b">
         <v>1</v>
@@ -4062,42 +3729,42 @@
         <v>1</v>
       </c>
       <c r="K69" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="L69" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="P69" t="s">
         <v>28</v>
       </c>
       <c r="Q69" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R69">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="S69">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B70" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D70" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F70" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G70" s="1" t="b">
         <v>0</v>
@@ -4112,42 +3779,42 @@
         <v>1</v>
       </c>
       <c r="K70" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="L70" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="P70" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R70">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="S70">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B71" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F71" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G71" s="1" t="b">
         <v>1</v>
@@ -4162,42 +3829,42 @@
         <v>1</v>
       </c>
       <c r="K71" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="L71" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="P71" t="s">
         <v>20</v>
       </c>
-      <c r="Q71" s="2" t="s">
-        <v>78</v>
+      <c r="Q71" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="R71">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="S71">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E72" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F72" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G72" s="1" t="b">
         <v>0</v>
@@ -4212,42 +3879,42 @@
         <v>1</v>
       </c>
       <c r="K72" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="L72" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="P72" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q72" s="5" t="s">
-        <v>71</v>
+        <v>24</v>
+      </c>
+      <c r="Q72" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R72">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="S72">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E73" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G73" s="1" t="b">
         <v>1</v>
@@ -4262,42 +3929,42 @@
         <v>1</v>
       </c>
       <c r="K73" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="L73" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="P73" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="R73">
-        <v>542</v>
+        <v>530</v>
       </c>
       <c r="S73">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D74" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E74" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F74" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G74" s="1" t="b">
         <v>0</v>
@@ -4312,43 +3979,43 @@
         <v>1</v>
       </c>
       <c r="K74" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="L74" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="P74" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="R74">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="S74">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D75" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F75" t="s">
         <v>47</v>
       </c>
-      <c r="F75" t="s">
-        <v>38</v>
-      </c>
       <c r="G75" s="1" t="b">
         <v>1</v>
       </c>
@@ -4362,94 +4029,680 @@
         <v>1</v>
       </c>
       <c r="K75" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="L75" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="P75" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R75">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="S75">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D76" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+      <c r="G76" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" t="b">
+        <v>1</v>
+      </c>
+      <c r="K76" t="s">
+        <v>178</v>
+      </c>
+      <c r="L76" t="s">
+        <v>224</v>
+      </c>
+      <c r="P76" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R76">
+        <v>533</v>
+      </c>
+      <c r="S76">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D77" t="s">
+        <v>142</v>
+      </c>
+      <c r="E77" t="s">
+        <v>36</v>
+      </c>
+      <c r="F77" t="s">
+        <v>23</v>
+      </c>
+      <c r="G77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="b">
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
+      <c r="K77" t="s">
+        <v>179</v>
+      </c>
+      <c r="L77" t="s">
+        <v>225</v>
+      </c>
+      <c r="P77" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R77">
+        <v>534</v>
+      </c>
+      <c r="S77">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" t="s">
+        <v>135</v>
+      </c>
+      <c r="D78" t="s">
+        <v>142</v>
+      </c>
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>23</v>
+      </c>
+      <c r="G78" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" t="b">
+        <v>1</v>
+      </c>
+      <c r="K78" t="s">
+        <v>180</v>
+      </c>
+      <c r="L78" t="s">
+        <v>226</v>
+      </c>
+      <c r="P78" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q78" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R78">
+        <v>535</v>
+      </c>
+      <c r="S78">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" t="s">
+        <v>37</v>
+      </c>
+      <c r="G79" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H79" t="b">
+        <v>1</v>
+      </c>
+      <c r="I79" t="b">
+        <v>0</v>
+      </c>
+      <c r="J79" t="b">
+        <v>1</v>
+      </c>
+      <c r="K79" t="s">
+        <v>181</v>
+      </c>
+      <c r="L79" t="s">
+        <v>227</v>
+      </c>
+      <c r="P79" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q79" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="R79">
+        <v>536</v>
+      </c>
+      <c r="S79">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" t="s">
+        <v>142</v>
+      </c>
+      <c r="E80" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80" t="s">
+        <v>37</v>
+      </c>
+      <c r="G80" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="b">
+        <v>1</v>
+      </c>
+      <c r="K80" t="s">
+        <v>182</v>
+      </c>
+      <c r="L80" t="s">
+        <v>228</v>
+      </c>
+      <c r="P80" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q80" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R80">
+        <v>537</v>
+      </c>
+      <c r="S80">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" t="s">
+        <v>124</v>
+      </c>
+      <c r="C81" t="s">
+        <v>136</v>
+      </c>
+      <c r="D81" t="s">
+        <v>143</v>
+      </c>
+      <c r="E81" t="s">
+        <v>36</v>
+      </c>
+      <c r="F81" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+      <c r="K81" t="s">
+        <v>183</v>
+      </c>
+      <c r="L81" t="s">
+        <v>229</v>
+      </c>
+      <c r="P81" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q81" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R81">
+        <v>538</v>
+      </c>
+      <c r="S81">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" t="s">
+        <v>125</v>
+      </c>
+      <c r="C82" t="s">
+        <v>136</v>
+      </c>
+      <c r="D82" t="s">
+        <v>143</v>
+      </c>
+      <c r="E82" t="s">
+        <v>36</v>
+      </c>
+      <c r="F82" t="s">
         <v>47</v>
       </c>
-      <c r="F76" t="s">
-        <v>38</v>
-      </c>
-      <c r="G76" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76" t="b">
-        <v>0</v>
-      </c>
-      <c r="I76" t="b">
-        <v>1</v>
-      </c>
-      <c r="J76" t="b">
-        <v>1</v>
-      </c>
-      <c r="K76" t="s">
-        <v>191</v>
-      </c>
-      <c r="L76" t="s">
-        <v>237</v>
-      </c>
-      <c r="P76" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q76" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="R76">
+      <c r="G82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="b">
+        <v>1</v>
+      </c>
+      <c r="K82" t="s">
+        <v>184</v>
+      </c>
+      <c r="L82" t="s">
+        <v>230</v>
+      </c>
+      <c r="P82" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R82">
+        <v>539</v>
+      </c>
+      <c r="S82">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" t="s">
+        <v>143</v>
+      </c>
+      <c r="E83" t="s">
+        <v>22</v>
+      </c>
+      <c r="F83" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="b">
+        <v>0</v>
+      </c>
+      <c r="J83" t="b">
+        <v>1</v>
+      </c>
+      <c r="K83" t="s">
+        <v>185</v>
+      </c>
+      <c r="L83" t="s">
+        <v>231</v>
+      </c>
+      <c r="P83" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q83" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R83">
+        <v>540</v>
+      </c>
+      <c r="S83">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" t="s">
+        <v>127</v>
+      </c>
+      <c r="C84" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" t="s">
+        <v>22</v>
+      </c>
+      <c r="F84" t="s">
+        <v>37</v>
+      </c>
+      <c r="G84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="b">
+        <v>1</v>
+      </c>
+      <c r="K84" t="s">
+        <v>186</v>
+      </c>
+      <c r="L84" t="s">
+        <v>232</v>
+      </c>
+      <c r="P84" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q84" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="R84">
+        <v>541</v>
+      </c>
+      <c r="S84">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K85" t="s">
+        <v>187</v>
+      </c>
+      <c r="L85" t="s">
+        <v>233</v>
+      </c>
+      <c r="P85" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R85">
+        <v>542</v>
+      </c>
+      <c r="S85">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" t="s">
+        <v>129</v>
+      </c>
+      <c r="C86" t="s">
+        <v>137</v>
+      </c>
+      <c r="D86" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" t="s">
+        <v>23</v>
+      </c>
+      <c r="G86" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" t="b">
+        <v>1</v>
+      </c>
+      <c r="K86" t="s">
+        <v>188</v>
+      </c>
+      <c r="L86" t="s">
+        <v>234</v>
+      </c>
+      <c r="P86" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q86" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R86">
+        <v>543</v>
+      </c>
+      <c r="S86">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" t="s">
+        <v>144</v>
+      </c>
+      <c r="E87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" t="s">
+        <v>37</v>
+      </c>
+      <c r="G87" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H87" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" t="b">
+        <v>1</v>
+      </c>
+      <c r="K87" t="s">
+        <v>189</v>
+      </c>
+      <c r="L87" t="s">
+        <v>235</v>
+      </c>
+      <c r="P87" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R87">
+        <v>544</v>
+      </c>
+      <c r="S87">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>131</v>
+      </c>
+      <c r="B88" t="s">
+        <v>131</v>
+      </c>
+      <c r="C88" t="s">
+        <v>137</v>
+      </c>
+      <c r="D88" t="s">
+        <v>144</v>
+      </c>
+      <c r="E88" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" t="b">
+        <v>1</v>
+      </c>
+      <c r="K88" t="s">
+        <v>190</v>
+      </c>
+      <c r="L88" t="s">
+        <v>236</v>
+      </c>
+      <c r="P88" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q88" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R88">
         <v>545</v>
       </c>
-      <c r="S76">
+      <c r="S88">
         <v>105</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G77" s="1"/>
-      <c r="Q77" s="5"/>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="G78" s="1"/>
-      <c r="Q78" s="2"/>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q79" s="5"/>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q80" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="T19" r:id="rId2"/>
-    <hyperlink ref="L25" r:id="rId3"/>
-    <hyperlink ref="T26" r:id="rId4"/>
+    <hyperlink ref="T31" r:id="rId1"/>
+    <hyperlink ref="L37" r:id="rId2"/>
+    <hyperlink ref="T38" r:id="rId3"/>
+    <hyperlink ref="L2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>